<commit_message>
CNA analysis update:     * RBS-ATrgetsAnalysis-CNA spread sheet: calculated Sn and Al thickness for the targets used in each irradiation (need to improve calculations taking into account the beam energy loss in the different layers of the target);     * Beam current monitor files: added files missing 240712{1-10}-SI2.txt (need to upload them into Notion and lstore);     * CrossSection.py: corrected units in the Rutherford differential cross-section calculation;     * Plot_Accumulation_Ge.py and Fits.py: improved methods to fit N_Dirr from the Npeak(t_acqui) function (still need to implement minor improvements);
</commit_message>
<xml_diff>
--- a/CNA/RBS-TargetsAnalysis-CNA.xlsx
+++ b/CNA/RBS-TargetsAnalysis-CNA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7310" tabRatio="668"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7305" tabRatio="668"/>
   </bookViews>
   <sheets>
     <sheet name="Sn+Al targets" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="37">
   <si>
     <t>g/cm^3</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>116Sn-G1</t>
+  </si>
+  <si>
+    <t>116Sn-D8</t>
+  </si>
+  <si>
+    <t>116Sn-D5</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -847,6 +853,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,11 +1146,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2013588640"/>
-        <c:axId val="-2013603872"/>
+        <c:axId val="-1721889552"/>
+        <c:axId val="-1721890640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2013588640"/>
+        <c:axId val="-1721889552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,12 +1263,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2013603872"/>
+        <c:crossAx val="-1721890640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2013603872"/>
+        <c:axId val="-1721890640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1381,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2013588640"/>
+        <c:crossAx val="-1721889552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1589,11 +1598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2014410992"/>
-        <c:axId val="-1752292576"/>
+        <c:axId val="-1721894992"/>
+        <c:axId val="-1721888464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2014410992"/>
+        <c:axId val="-1721894992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,12 +1715,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752292576"/>
+        <c:crossAx val="-1721888464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1752292576"/>
+        <c:axId val="-1721888464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +1833,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2014410992"/>
+        <c:crossAx val="-1721894992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2041,11 +2050,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1752284416"/>
-        <c:axId val="-1752288768"/>
+        <c:axId val="-1721885200"/>
+        <c:axId val="-1721897168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1752284416"/>
+        <c:axId val="-1721885200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,12 +2167,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752288768"/>
+        <c:crossAx val="-1721897168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1752288768"/>
+        <c:axId val="-1721897168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2285,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752284416"/>
+        <c:crossAx val="-1721885200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2493,11 +2502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1752293120"/>
-        <c:axId val="-1752295840"/>
+        <c:axId val="-1721887920"/>
+        <c:axId val="-1721898800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1752293120"/>
+        <c:axId val="-1721887920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,12 +2619,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752295840"/>
+        <c:crossAx val="-1721898800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1752295840"/>
+        <c:axId val="-1721898800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,7 +2737,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752293120"/>
+        <c:crossAx val="-1721887920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2881,12 +2890,88 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17203905320490975"/>
+                  <c:y val="-0.24307086787793261"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sn+Al targets'!$L$81:$L$86</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>317.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>346.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>434</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2927,11 +3012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1752295296"/>
-        <c:axId val="-1752297472"/>
+        <c:axId val="-1721898256"/>
+        <c:axId val="-1721886832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1752295296"/>
+        <c:axId val="-1721898256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,12 +3129,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752297472"/>
+        <c:crossAx val="-1721886832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1752297472"/>
+        <c:axId val="-1721886832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3247,509 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1752295296"/>
+        <c:crossAx val="-1721898256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RBS Calib Ebeam = 5.0 MeV</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>RBS Calib Ebeam = 5.0 MeV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11411547360680142"/>
+                  <c:y val="-0.22924789016330568"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sn+Al targets'!$L$100:$L$105</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>370.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>413.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>463.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>472</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sn+Al targets'!$K$100:$K$105</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3601.3603252040011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3909.289944099171</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4321.6528739353071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4346.6455203510932</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4833.3595556669889</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4900.2426588796607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1602602544"/>
+        <c:axId val="-1602608528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1602602544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1200" b="1"/>
+                  <a:t>Channel</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1602608528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1602608528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1200" b="1"/>
+                  <a:t>Energy (keV)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1602602544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3411,6 +3998,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5476,6 +6103,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6146,6 +7289,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6417,56 +7592,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X96"/>
+  <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.26953125" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.453125" customWidth="1"/>
-    <col min="19" max="19" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1796875" customWidth="1"/>
-    <col min="22" max="22" width="8.1796875" customWidth="1"/>
-    <col min="23" max="23" width="8.54296875" customWidth="1"/>
-    <col min="24" max="24" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12" customWidth="1"/>
-    <col min="27" max="27" width="8.1796875" customWidth="1"/>
-    <col min="28" max="28" width="11.7265625" customWidth="1"/>
-    <col min="29" max="29" width="14.54296875" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.26953125" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.81640625" customWidth="1"/>
-    <col min="38" max="39" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.1796875" customWidth="1"/>
-    <col min="42" max="42" width="6.453125" customWidth="1"/>
-    <col min="43" max="44" width="8.453125" customWidth="1"/>
-    <col min="45" max="45" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.28515625" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" customWidth="1"/>
+    <col min="38" max="39" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.140625" customWidth="1"/>
+    <col min="42" max="42" width="6.42578125" customWidth="1"/>
+    <col min="43" max="44" width="8.42578125" customWidth="1"/>
+    <col min="45" max="45" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>15</v>
       </c>
@@ -6486,8 +7661,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="72"/>
       <c r="C3" s="73"/>
       <c r="D3" s="73"/>
@@ -6512,7 +7687,7 @@
       <c r="W3" s="73"/>
       <c r="X3" s="74"/>
     </row>
-    <row r="4" spans="1:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="C4" s="69" t="s">
         <v>28</v>
@@ -6555,7 +7730,7 @@
       <c r="W4" s="37"/>
       <c r="X4" s="38"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" s="36"/>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
@@ -6594,7 +7769,7 @@
       <c r="W5" s="37"/>
       <c r="X5" s="38"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" s="36"/>
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
@@ -6633,7 +7808,7 @@
       <c r="W6" s="37"/>
       <c r="X6" s="38"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
       <c r="D7" s="37">
@@ -6677,7 +7852,7 @@
       <c r="W7" s="37"/>
       <c r="X7" s="38"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="36"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37">
@@ -6720,7 +7895,7 @@
       <c r="W8" s="37"/>
       <c r="X8" s="38"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="36"/>
       <c r="C9" s="37"/>
       <c r="D9" s="37">
@@ -6763,7 +7938,7 @@
       <c r="W9" s="37"/>
       <c r="X9" s="38"/>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="36"/>
       <c r="C10" s="37"/>
       <c r="D10" s="37">
@@ -6806,7 +7981,7 @@
       <c r="W10" s="37"/>
       <c r="X10" s="38"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="36"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -6851,7 +8026,7 @@
       </c>
       <c r="X11" s="38"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12" s="36"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -6902,7 +8077,7 @@
       </c>
       <c r="X12" s="38"/>
     </row>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
@@ -6927,7 +8102,7 @@
       <c r="W13" s="37"/>
       <c r="X13" s="38"/>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36"/>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -6952,7 +8127,7 @@
       <c r="W14" s="37"/>
       <c r="X14" s="38"/>
     </row>
-    <row r="15" spans="1:24" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36"/>
       <c r="C15" s="37"/>
       <c r="D15" s="37"/>
@@ -6995,7 +8170,7 @@
       </c>
       <c r="X15" s="38"/>
     </row>
-    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36"/>
       <c r="C16" s="37"/>
       <c r="D16" s="37"/>
@@ -7040,7 +8215,7 @@
       </c>
       <c r="X16" s="38"/>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="36"/>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
@@ -7067,7 +8242,7 @@
       <c r="W17" s="37"/>
       <c r="X17" s="38"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="36"/>
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
@@ -7092,7 +8267,7 @@
       <c r="W18" s="37"/>
       <c r="X18" s="38"/>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="36"/>
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
@@ -7117,7 +8292,7 @@
       <c r="W19" s="37"/>
       <c r="X19" s="38"/>
     </row>
-    <row r="20" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="75"/>
       <c r="C20" s="76"/>
       <c r="D20" s="76"/>
@@ -7142,8 +8317,8 @@
       <c r="W20" s="76"/>
       <c r="X20" s="77"/>
     </row>
-    <row r="21" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="72"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
@@ -7168,7 +8343,7 @@
       <c r="W22" s="73"/>
       <c r="X22" s="74"/>
     </row>
-    <row r="23" spans="2:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36"/>
       <c r="C23" s="69" t="s">
         <v>28</v>
@@ -7211,7 +8386,7 @@
       <c r="W23" s="37"/>
       <c r="X23" s="38"/>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="36"/>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
@@ -7250,7 +8425,7 @@
       <c r="W24" s="37"/>
       <c r="X24" s="38"/>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="36"/>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -7289,7 +8464,7 @@
       <c r="W25" s="37"/>
       <c r="X25" s="38"/>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="36"/>
       <c r="C26" s="37"/>
       <c r="D26" s="37">
@@ -7333,7 +8508,7 @@
       <c r="W26" s="37"/>
       <c r="X26" s="38"/>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="36"/>
       <c r="C27" s="37"/>
       <c r="D27" s="37">
@@ -7376,7 +8551,7 @@
       <c r="W27" s="37"/>
       <c r="X27" s="38"/>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="36"/>
       <c r="C28" s="37"/>
       <c r="D28" s="37">
@@ -7419,7 +8594,7 @@
       <c r="W28" s="37"/>
       <c r="X28" s="38"/>
     </row>
-    <row r="29" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36"/>
       <c r="C29" s="37"/>
       <c r="D29" s="37">
@@ -7462,7 +8637,7 @@
       <c r="W29" s="37"/>
       <c r="X29" s="38"/>
     </row>
-    <row r="30" spans="2:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36"/>
       <c r="C30" s="37"/>
       <c r="D30" s="37"/>
@@ -7507,7 +8682,7 @@
       </c>
       <c r="X30" s="38"/>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="36"/>
       <c r="C31" s="37"/>
       <c r="D31" s="37"/>
@@ -7558,7 +8733,7 @@
       </c>
       <c r="X31" s="38"/>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="36"/>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
@@ -7583,7 +8758,7 @@
       <c r="W32" s="37"/>
       <c r="X32" s="38"/>
     </row>
-    <row r="33" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="36"/>
       <c r="C33" s="37"/>
       <c r="D33" s="37"/>
@@ -7608,7 +8783,7 @@
       <c r="W33" s="37"/>
       <c r="X33" s="38"/>
     </row>
-    <row r="34" spans="2:24" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="36"/>
       <c r="C34" s="37"/>
       <c r="D34" s="37"/>
@@ -7651,7 +8826,7 @@
       </c>
       <c r="X34" s="38"/>
     </row>
-    <row r="35" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="36"/>
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
@@ -7696,7 +8871,7 @@
       </c>
       <c r="X35" s="38"/>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
       <c r="C36" s="37"/>
       <c r="D36" s="37"/>
@@ -7723,7 +8898,7 @@
       <c r="W36" s="37"/>
       <c r="X36" s="38"/>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="36"/>
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
@@ -7748,7 +8923,7 @@
       <c r="W37" s="37"/>
       <c r="X37" s="38"/>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="36"/>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
@@ -7773,7 +8948,7 @@
       <c r="W38" s="37"/>
       <c r="X38" s="38"/>
     </row>
-    <row r="39" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="75"/>
       <c r="C39" s="76"/>
       <c r="D39" s="76"/>
@@ -7798,8 +8973,8 @@
       <c r="W39" s="76"/>
       <c r="X39" s="77"/>
     </row>
-    <row r="40" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="72"/>
       <c r="C41" s="73"/>
       <c r="D41" s="73"/>
@@ -7824,7 +8999,7 @@
       <c r="W41" s="73"/>
       <c r="X41" s="74"/>
     </row>
-    <row r="42" spans="2:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="36"/>
       <c r="C42" s="69" t="s">
         <v>28</v>
@@ -7867,7 +9042,7 @@
       <c r="W42" s="37"/>
       <c r="X42" s="38"/>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B43" s="36"/>
       <c r="C43" s="37"/>
       <c r="D43" s="37"/>
@@ -7906,7 +9081,7 @@
       <c r="W43" s="37"/>
       <c r="X43" s="38"/>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" s="36"/>
       <c r="C44" s="37"/>
       <c r="D44" s="37"/>
@@ -7945,7 +9120,7 @@
       <c r="W44" s="37"/>
       <c r="X44" s="38"/>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" s="36"/>
       <c r="C45" s="37"/>
       <c r="D45" s="37">
@@ -7989,7 +9164,7 @@
       <c r="W45" s="37"/>
       <c r="X45" s="38"/>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" s="36"/>
       <c r="C46" s="37"/>
       <c r="D46" s="37">
@@ -8032,7 +9207,7 @@
       <c r="W46" s="37"/>
       <c r="X46" s="38"/>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="36"/>
       <c r="C47" s="37"/>
       <c r="D47" s="37">
@@ -8075,7 +9250,7 @@
       <c r="W47" s="37"/>
       <c r="X47" s="38"/>
     </row>
-    <row r="48" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="36"/>
       <c r="C48" s="37"/>
       <c r="D48" s="37">
@@ -8118,7 +9293,7 @@
       <c r="W48" s="37"/>
       <c r="X48" s="38"/>
     </row>
-    <row r="49" spans="2:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="36"/>
       <c r="C49" s="37"/>
       <c r="D49" s="37"/>
@@ -8163,7 +9338,7 @@
       </c>
       <c r="X49" s="38"/>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B50" s="36"/>
       <c r="C50" s="37"/>
       <c r="D50" s="37"/>
@@ -8214,7 +9389,7 @@
       </c>
       <c r="X50" s="38"/>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B51" s="36"/>
       <c r="C51" s="37"/>
       <c r="D51" s="37"/>
@@ -8239,7 +9414,7 @@
       <c r="W51" s="37"/>
       <c r="X51" s="38"/>
     </row>
-    <row r="52" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="36"/>
       <c r="C52" s="37"/>
       <c r="D52" s="37"/>
@@ -8264,7 +9439,7 @@
       <c r="W52" s="37"/>
       <c r="X52" s="38"/>
     </row>
-    <row r="53" spans="2:24" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="36"/>
       <c r="C53" s="37"/>
       <c r="D53" s="37"/>
@@ -8307,7 +9482,7 @@
       </c>
       <c r="X53" s="38"/>
     </row>
-    <row r="54" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="36"/>
       <c r="C54" s="37"/>
       <c r="D54" s="37"/>
@@ -8352,7 +9527,7 @@
       </c>
       <c r="X54" s="38"/>
     </row>
-    <row r="55" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55" s="36"/>
       <c r="C55" s="37"/>
       <c r="D55" s="37"/>
@@ -8379,7 +9554,7 @@
       <c r="W55" s="37"/>
       <c r="X55" s="38"/>
     </row>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B56" s="36"/>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
@@ -8404,7 +9579,7 @@
       <c r="W56" s="37"/>
       <c r="X56" s="38"/>
     </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" s="36"/>
       <c r="C57" s="37"/>
       <c r="D57" s="37"/>
@@ -8429,7 +9604,7 @@
       <c r="W57" s="37"/>
       <c r="X57" s="38"/>
     </row>
-    <row r="58" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="75"/>
       <c r="C58" s="76"/>
       <c r="D58" s="76"/>
@@ -8454,8 +9629,8 @@
       <c r="W58" s="76"/>
       <c r="X58" s="77"/>
     </row>
-    <row r="59" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="60" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="72"/>
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
@@ -8480,7 +9655,7 @@
       <c r="W60" s="73"/>
       <c r="X60" s="74"/>
     </row>
-    <row r="61" spans="2:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="36"/>
       <c r="C61" s="69" t="s">
         <v>28</v>
@@ -8523,7 +9698,7 @@
       <c r="W61" s="37"/>
       <c r="X61" s="38"/>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B62" s="36"/>
       <c r="C62" s="37"/>
       <c r="D62" s="37"/>
@@ -8562,7 +9737,7 @@
       <c r="W62" s="37"/>
       <c r="X62" s="38"/>
     </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B63" s="36"/>
       <c r="C63" s="37"/>
       <c r="D63" s="37"/>
@@ -8601,7 +9776,7 @@
       <c r="W63" s="37"/>
       <c r="X63" s="38"/>
     </row>
-    <row r="64" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B64" s="36"/>
       <c r="C64" s="37"/>
       <c r="D64" s="37">
@@ -8645,7 +9820,7 @@
       <c r="W64" s="37"/>
       <c r="X64" s="38"/>
     </row>
-    <row r="65" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B65" s="36"/>
       <c r="C65" s="37"/>
       <c r="D65" s="37">
@@ -8688,7 +9863,7 @@
       <c r="W65" s="37"/>
       <c r="X65" s="38"/>
     </row>
-    <row r="66" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B66" s="36"/>
       <c r="C66" s="37"/>
       <c r="D66" s="37">
@@ -8731,7 +9906,7 @@
       <c r="W66" s="37"/>
       <c r="X66" s="38"/>
     </row>
-    <row r="67" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
       <c r="D67" s="37">
@@ -8774,7 +9949,7 @@
       <c r="W67" s="37"/>
       <c r="X67" s="38"/>
     </row>
-    <row r="68" spans="2:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="36"/>
       <c r="C68" s="37"/>
       <c r="D68" s="37"/>
@@ -8819,7 +9994,7 @@
       </c>
       <c r="X68" s="38"/>
     </row>
-    <row r="69" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B69" s="36"/>
       <c r="C69" s="37"/>
       <c r="D69" s="37"/>
@@ -8870,7 +10045,7 @@
       </c>
       <c r="X69" s="38"/>
     </row>
-    <row r="70" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B70" s="36"/>
       <c r="C70" s="37"/>
       <c r="D70" s="37"/>
@@ -8895,7 +10070,7 @@
       <c r="W70" s="37"/>
       <c r="X70" s="38"/>
     </row>
-    <row r="71" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="36"/>
       <c r="C71" s="37"/>
       <c r="D71" s="37"/>
@@ -8920,7 +10095,7 @@
       <c r="W71" s="37"/>
       <c r="X71" s="38"/>
     </row>
-    <row r="72" spans="2:24" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="36"/>
       <c r="C72" s="37"/>
       <c r="D72" s="37"/>
@@ -8963,7 +10138,7 @@
       </c>
       <c r="X72" s="38"/>
     </row>
-    <row r="73" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="36"/>
       <c r="C73" s="37"/>
       <c r="D73" s="37"/>
@@ -9008,7 +10183,7 @@
       </c>
       <c r="X73" s="38"/>
     </row>
-    <row r="74" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B74" s="36"/>
       <c r="C74" s="37"/>
       <c r="D74" s="37"/>
@@ -9035,7 +10210,7 @@
       <c r="W74" s="37"/>
       <c r="X74" s="38"/>
     </row>
-    <row r="75" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B75" s="36"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -9060,7 +10235,7 @@
       <c r="W75" s="37"/>
       <c r="X75" s="38"/>
     </row>
-    <row r="76" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B76" s="36"/>
       <c r="C76" s="37"/>
       <c r="D76" s="37"/>
@@ -9085,7 +10260,7 @@
       <c r="W76" s="37"/>
       <c r="X76" s="38"/>
     </row>
-    <row r="77" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="75"/>
       <c r="C77" s="76"/>
       <c r="D77" s="76"/>
@@ -9110,8 +10285,8 @@
       <c r="W77" s="76"/>
       <c r="X77" s="77"/>
     </row>
-    <row r="78" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="79" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="72"/>
       <c r="C79" s="73"/>
       <c r="D79" s="73"/>
@@ -9136,7 +10311,7 @@
       <c r="W79" s="73"/>
       <c r="X79" s="74"/>
     </row>
-    <row r="80" spans="2:24" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="36"/>
       <c r="C80" s="69" t="s">
         <v>28</v>
@@ -9179,7 +10354,7 @@
       <c r="W80" s="37"/>
       <c r="X80" s="38"/>
     </row>
-    <row r="81" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B81" s="36"/>
       <c r="C81" s="37"/>
       <c r="D81" s="37"/>
@@ -9202,7 +10377,9 @@
         <f>$D$80*1000*J81</f>
         <v>3385.2787056917609</v>
       </c>
-      <c r="L81" s="60"/>
+      <c r="L81" s="60">
+        <v>317.5</v>
+      </c>
       <c r="M81" s="37"/>
       <c r="N81" s="37"/>
       <c r="O81" s="37"/>
@@ -9216,7 +10393,7 @@
       <c r="W81" s="37"/>
       <c r="X81" s="38"/>
     </row>
-    <row r="82" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B82" s="36"/>
       <c r="C82" s="37"/>
       <c r="D82" s="37"/>
@@ -9239,7 +10416,9 @@
         <f t="shared" ref="K82:K86" si="9">$D$80*1000*J82</f>
         <v>3674.7325474532204</v>
       </c>
-      <c r="L82" s="56"/>
+      <c r="L82" s="56">
+        <v>346.5</v>
+      </c>
       <c r="M82" s="37"/>
       <c r="N82" s="37"/>
       <c r="O82" s="37"/>
@@ -9253,7 +10432,7 @@
       <c r="W82" s="37"/>
       <c r="X82" s="38"/>
     </row>
-    <row r="83" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B83" s="36"/>
       <c r="C83" s="37"/>
       <c r="D83" s="37" t="e">
@@ -9281,7 +10460,9 @@
         <f t="shared" si="9"/>
         <v>4062.3537014991889</v>
       </c>
-      <c r="L83" s="32"/>
+      <c r="L83" s="32">
+        <v>378</v>
+      </c>
       <c r="M83" s="37"/>
       <c r="N83" s="37"/>
       <c r="O83" s="37"/>
@@ -9295,7 +10476,7 @@
       <c r="W83" s="37"/>
       <c r="X83" s="38"/>
     </row>
-    <row r="84" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B84" s="36"/>
       <c r="C84" s="37"/>
       <c r="D84" s="37" t="e">
@@ -9336,7 +10517,7 @@
       <c r="W84" s="37"/>
       <c r="X84" s="38"/>
     </row>
-    <row r="85" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B85" s="36"/>
       <c r="C85" s="37"/>
       <c r="D85" s="37" t="e">
@@ -9363,7 +10544,9 @@
         <f t="shared" si="9"/>
         <v>4543.3579823269692</v>
       </c>
-      <c r="L85" s="47"/>
+      <c r="L85" s="47">
+        <v>434</v>
+      </c>
       <c r="M85" s="37"/>
       <c r="N85" s="37"/>
       <c r="O85" s="37"/>
@@ -9377,7 +10560,7 @@
       <c r="W85" s="37"/>
       <c r="X85" s="38"/>
     </row>
-    <row r="86" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="36"/>
       <c r="C86" s="37"/>
       <c r="D86" s="37" t="e">
@@ -9418,7 +10601,7 @@
       <c r="W86" s="37"/>
       <c r="X86" s="38"/>
     </row>
-    <row r="87" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="36"/>
       <c r="C87" s="37"/>
       <c r="D87" s="37"/>
@@ -9463,7 +10646,7 @@
       </c>
       <c r="X87" s="38"/>
     </row>
-    <row r="88" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B88" s="36"/>
       <c r="C88" s="37"/>
       <c r="D88" s="37"/>
@@ -9475,38 +10658,46 @@
       <c r="J88" s="37"/>
       <c r="K88" s="37"/>
       <c r="L88" s="37"/>
-      <c r="M88" s="6"/>
+      <c r="M88" s="6">
+        <v>36.340000000000003</v>
+      </c>
       <c r="N88" s="15">
         <f>M88*$B$1/10</f>
-        <v>0</v>
-      </c>
-      <c r="O88" s="19"/>
+        <v>26.564540000000001</v>
+      </c>
+      <c r="O88" s="19">
+        <v>37.130000000000003</v>
+      </c>
       <c r="P88" s="6">
         <f>O88*$B$1/10</f>
-        <v>0</v>
+        <v>27.142029999999998</v>
       </c>
       <c r="Q88" s="18">
         <f>(($J$47/COS(RADIANS(0))*$N$88)+(1/COS(RADIANS(180-165))*$P$88))</f>
-        <v>0</v>
+        <v>53.778691797155474</v>
       </c>
       <c r="R88" s="37"/>
-      <c r="S88" s="26"/>
+      <c r="S88" s="26">
+        <v>61.11</v>
+      </c>
       <c r="T88" s="15">
         <f>S88*$E$1/10</f>
-        <v>0</v>
-      </c>
-      <c r="U88" s="26"/>
+        <v>16.493589</v>
+      </c>
+      <c r="U88" s="26">
+        <v>66.319999999999993</v>
+      </c>
       <c r="V88" s="6">
         <f>U88*$E$1/10</f>
-        <v>0</v>
+        <v>17.899767999999998</v>
       </c>
       <c r="W88" s="14">
         <f>(($J$45/COS(RADIANS(0))*T88)+(1/COS(RADIANS(180-165))*V88))</f>
-        <v>0</v>
+        <v>32.787116705938182</v>
       </c>
       <c r="X88" s="38"/>
     </row>
-    <row r="89" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B89" s="36"/>
       <c r="C89" s="37"/>
       <c r="D89" s="37"/>
@@ -9531,7 +10722,7 @@
       <c r="W89" s="37"/>
       <c r="X89" s="38"/>
     </row>
-    <row r="90" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="36"/>
       <c r="C90" s="37"/>
       <c r="D90" s="37"/>
@@ -9556,7 +10747,7 @@
       <c r="W90" s="37"/>
       <c r="X90" s="38"/>
     </row>
-    <row r="91" spans="2:24" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="36"/>
       <c r="C91" s="37"/>
       <c r="D91" s="37"/>
@@ -9569,7 +10760,7 @@
       <c r="K91" s="37"/>
       <c r="L91" s="37"/>
       <c r="M91" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>17</v>
@@ -9599,7 +10790,7 @@
       </c>
       <c r="X91" s="38"/>
     </row>
-    <row r="92" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="36"/>
       <c r="C92" s="37"/>
       <c r="D92" s="37"/>
@@ -9612,31 +10803,39 @@
       <c r="K92" s="37"/>
       <c r="L92" s="37"/>
       <c r="M92" s="27"/>
-      <c r="N92" s="20"/>
-      <c r="O92" s="21"/>
-      <c r="P92" s="25" t="e">
-        <f>(N92-O92)*D83</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q92" s="23" t="e">
+      <c r="N92" s="20">
+        <v>434</v>
+      </c>
+      <c r="O92" s="21">
+        <v>425.5</v>
+      </c>
+      <c r="P92" s="25">
+        <f>(N92-O92)*10.028</f>
+        <v>85.238</v>
+      </c>
+      <c r="Q92" s="23">
         <f>P92*10^3/$Q$88</f>
-        <v>#VALUE!</v>
+        <v>1584.9771935974929</v>
       </c>
       <c r="R92" s="37"/>
       <c r="S92" s="24"/>
-      <c r="T92" s="20"/>
-      <c r="U92" s="21"/>
-      <c r="V92" s="22" t="e">
-        <f>(T92-U92)*D83</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W92" s="23" t="e">
+      <c r="T92" s="20">
+        <v>378</v>
+      </c>
+      <c r="U92" s="21">
+        <v>373.5</v>
+      </c>
+      <c r="V92" s="22">
+        <f>(T92-U92)*10.028</f>
+        <v>45.126000000000005</v>
+      </c>
+      <c r="W92" s="23">
         <f>V92*10^3/$W$88</f>
-        <v>#VALUE!</v>
+        <v>1376.3332837323596</v>
       </c>
       <c r="X92" s="38"/>
     </row>
-    <row r="93" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B93" s="36"/>
       <c r="C93" s="37"/>
       <c r="D93" s="37"/>
@@ -9663,7 +10862,7 @@
       <c r="W93" s="37"/>
       <c r="X93" s="38"/>
     </row>
-    <row r="94" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B94" s="36"/>
       <c r="C94" s="37"/>
       <c r="D94" s="37"/>
@@ -9688,7 +10887,7 @@
       <c r="W94" s="37"/>
       <c r="X94" s="38"/>
     </row>
-    <row r="95" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B95" s="36"/>
       <c r="C95" s="37"/>
       <c r="D95" s="37"/>
@@ -9713,7 +10912,7 @@
       <c r="W95" s="37"/>
       <c r="X95" s="38"/>
     </row>
-    <row r="96" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="75"/>
       <c r="C96" s="76"/>
       <c r="D96" s="76"/>
@@ -9738,6 +10937,662 @@
       <c r="W96" s="76"/>
       <c r="X96" s="77"/>
     </row>
+    <row r="97" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="72"/>
+      <c r="C98" s="73"/>
+      <c r="D98" s="73"/>
+      <c r="E98" s="73"/>
+      <c r="F98" s="73"/>
+      <c r="G98" s="73"/>
+      <c r="H98" s="73"/>
+      <c r="I98" s="73"/>
+      <c r="J98" s="73"/>
+      <c r="K98" s="73"/>
+      <c r="L98" s="73"/>
+      <c r="M98" s="73"/>
+      <c r="N98" s="73"/>
+      <c r="O98" s="73"/>
+      <c r="P98" s="73"/>
+      <c r="Q98" s="73"/>
+      <c r="R98" s="73"/>
+      <c r="S98" s="73"/>
+      <c r="T98" s="73"/>
+      <c r="U98" s="73"/>
+      <c r="V98" s="73"/>
+      <c r="W98" s="73"/>
+      <c r="X98" s="74"/>
+    </row>
+    <row r="99" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="36"/>
+      <c r="C99" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D99" s="78">
+        <v>5</v>
+      </c>
+      <c r="E99" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F99" s="37"/>
+      <c r="G99" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H99" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I99" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J99" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="L99" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="M99" s="37"/>
+      <c r="N99" s="37"/>
+      <c r="O99" s="37"/>
+      <c r="P99" s="37"/>
+      <c r="Q99" s="37"/>
+      <c r="R99" s="37"/>
+      <c r="S99" s="37"/>
+      <c r="T99" s="37"/>
+      <c r="U99" s="37"/>
+      <c r="V99" s="37"/>
+      <c r="W99" s="37"/>
+      <c r="X99" s="38"/>
+    </row>
+    <row r="100" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B100" s="36"/>
+      <c r="C100" s="37"/>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="H100" s="58">
+        <v>6</v>
+      </c>
+      <c r="I100" s="58">
+        <v>12.010999999999999</v>
+      </c>
+      <c r="J100" s="59">
+        <f>((SQRT(1-(1/I100)^2*SIN(RADIANS(165))^2)+1/I100*COS(RADIANS(165)))/(1+1/I100))^2</f>
+        <v>0.72027206504080021</v>
+      </c>
+      <c r="K100" s="63">
+        <f>$D$99*1000*J100</f>
+        <v>3601.3603252040011</v>
+      </c>
+      <c r="L100" s="60">
+        <v>339</v>
+      </c>
+      <c r="M100" s="37"/>
+      <c r="N100" s="37"/>
+      <c r="O100" s="37"/>
+      <c r="P100" s="37"/>
+      <c r="Q100" s="37"/>
+      <c r="R100" s="37"/>
+      <c r="S100" s="37"/>
+      <c r="T100" s="37"/>
+      <c r="U100" s="37"/>
+      <c r="V100" s="37"/>
+      <c r="W100" s="37"/>
+      <c r="X100" s="38"/>
+    </row>
+    <row r="101" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B101" s="36"/>
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H101" s="53">
+        <v>8</v>
+      </c>
+      <c r="I101" s="54">
+        <v>15.999000000000001</v>
+      </c>
+      <c r="J101" s="55">
+        <f t="shared" ref="J101:J103" si="10">((SQRT(1-(1/I101)^2*SIN(RADIANS(165))^2)+1/I101*COS(RADIANS(165)))/(1+1/I101))^2</f>
+        <v>0.78185798881983415</v>
+      </c>
+      <c r="K101" s="64">
+        <f t="shared" ref="K101:K105" si="11">$D$99*1000*J101</f>
+        <v>3909.289944099171</v>
+      </c>
+      <c r="L101" s="56">
+        <v>370.5</v>
+      </c>
+      <c r="M101" s="37"/>
+      <c r="N101" s="37"/>
+      <c r="O101" s="37"/>
+      <c r="P101" s="37"/>
+      <c r="Q101" s="37"/>
+      <c r="R101" s="37"/>
+      <c r="S101" s="37"/>
+      <c r="T101" s="37"/>
+      <c r="U101" s="37"/>
+      <c r="V101" s="37"/>
+      <c r="W101" s="37"/>
+      <c r="X101" s="38"/>
+    </row>
+    <row r="102" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B102" s="36"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37">
+        <f t="array" ref="D102:E105">LINEST(K100:K105,L100:L105,TRUE,TRUE)</f>
+        <v>9.80127738708428</v>
+      </c>
+      <c r="E102" s="37">
+        <v>294.51733917568345</v>
+      </c>
+      <c r="F102" s="37"/>
+      <c r="G102" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H102" s="30">
+        <v>13</v>
+      </c>
+      <c r="I102" s="30">
+        <v>26.98</v>
+      </c>
+      <c r="J102" s="51">
+        <f t="shared" si="10"/>
+        <v>0.86433057478706143</v>
+      </c>
+      <c r="K102" s="65">
+        <f t="shared" si="11"/>
+        <v>4321.6528739353071</v>
+      </c>
+      <c r="L102" s="32">
+        <v>405</v>
+      </c>
+      <c r="M102" s="37"/>
+      <c r="N102" s="37"/>
+      <c r="O102" s="37"/>
+      <c r="P102" s="37"/>
+      <c r="Q102" s="37"/>
+      <c r="R102" s="37"/>
+      <c r="S102" s="37"/>
+      <c r="T102" s="37"/>
+      <c r="U102" s="37"/>
+      <c r="V102" s="37"/>
+      <c r="W102" s="37"/>
+      <c r="X102" s="38"/>
+    </row>
+    <row r="103" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B103" s="36"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37">
+        <v>0.28321744167471208</v>
+      </c>
+      <c r="E103" s="37">
+        <v>117.04882382677867</v>
+      </c>
+      <c r="F103" s="37"/>
+      <c r="G103" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="H103" s="40">
+        <v>14</v>
+      </c>
+      <c r="I103" s="40">
+        <v>28.09</v>
+      </c>
+      <c r="J103" s="49">
+        <f t="shared" si="10"/>
+        <v>0.86932910407021868</v>
+      </c>
+      <c r="K103" s="66">
+        <f t="shared" si="11"/>
+        <v>4346.6455203510932</v>
+      </c>
+      <c r="L103" s="41">
+        <v>413.5</v>
+      </c>
+      <c r="M103" s="37"/>
+      <c r="N103" s="37"/>
+      <c r="O103" s="37"/>
+      <c r="P103" s="37"/>
+      <c r="Q103" s="37"/>
+      <c r="R103" s="37"/>
+      <c r="S103" s="37"/>
+      <c r="T103" s="37"/>
+      <c r="U103" s="37"/>
+      <c r="V103" s="37"/>
+      <c r="W103" s="37"/>
+      <c r="X103" s="38"/>
+    </row>
+    <row r="104" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B104" s="36"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37">
+        <v>0.99667120895590811</v>
+      </c>
+      <c r="E104" s="37">
+        <v>32.714628413016257</v>
+      </c>
+      <c r="F104" s="37"/>
+      <c r="G104" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="H104" s="42">
+        <v>50</v>
+      </c>
+      <c r="I104" s="42">
+        <v>116</v>
+      </c>
+      <c r="J104" s="43">
+        <f>((SQRT(1-(1/I104)^2*SIN(RADIANS(165))^2)+1/I104*COS(RADIANS(165)))/(1+1/I104))^2</f>
+        <v>0.96667191113339779</v>
+      </c>
+      <c r="K104" s="67">
+        <f t="shared" si="11"/>
+        <v>4833.3595556669889</v>
+      </c>
+      <c r="L104" s="47">
+        <v>463.5</v>
+      </c>
+      <c r="M104" s="37"/>
+      <c r="N104" s="37"/>
+      <c r="O104" s="37"/>
+      <c r="P104" s="37"/>
+      <c r="Q104" s="37"/>
+      <c r="R104" s="37"/>
+      <c r="S104" s="37"/>
+      <c r="T104" s="37"/>
+      <c r="U104" s="37"/>
+      <c r="V104" s="37"/>
+      <c r="W104" s="37"/>
+      <c r="X104" s="38"/>
+    </row>
+    <row r="105" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="36"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="37">
+        <v>1197.637455465825</v>
+      </c>
+      <c r="E105" s="37">
+        <v>4</v>
+      </c>
+      <c r="F105" s="37"/>
+      <c r="G105" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="H105" s="46">
+        <v>78</v>
+      </c>
+      <c r="I105" s="46">
+        <v>195.1</v>
+      </c>
+      <c r="J105" s="50">
+        <f>((SQRT(1-(1/I105)^2*SIN(RADIANS(165))^2)+1/I105*COS(RADIANS(165)))/(1+1/I105))^2</f>
+        <v>0.9800485317759321</v>
+      </c>
+      <c r="K105" s="68">
+        <f t="shared" si="11"/>
+        <v>4900.2426588796607</v>
+      </c>
+      <c r="L105" s="48">
+        <v>472</v>
+      </c>
+      <c r="M105" s="37"/>
+      <c r="N105" s="37"/>
+      <c r="O105" s="37"/>
+      <c r="P105" s="37"/>
+      <c r="Q105" s="37"/>
+      <c r="R105" s="37"/>
+      <c r="S105" s="37"/>
+      <c r="T105" s="37"/>
+      <c r="U105" s="37"/>
+      <c r="V105" s="37"/>
+      <c r="W105" s="37"/>
+      <c r="X105" s="38"/>
+    </row>
+    <row r="106" spans="2:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="36"/>
+      <c r="C106" s="37"/>
+      <c r="D106" s="37"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="37"/>
+      <c r="K106" s="37"/>
+      <c r="L106" s="37"/>
+      <c r="M106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N106" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P106" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R106" s="37"/>
+      <c r="S106" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T106" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="U106" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="V106" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W106" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="X106" s="38"/>
+    </row>
+    <row r="107" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B107" s="36"/>
+      <c r="C107" s="37"/>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="37"/>
+      <c r="K107" s="37"/>
+      <c r="L107" s="37"/>
+      <c r="M107" s="6">
+        <v>34.93</v>
+      </c>
+      <c r="N107" s="15">
+        <f>M107*$B$1/10</f>
+        <v>25.533829999999998</v>
+      </c>
+      <c r="O107" s="19">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="P107" s="6">
+        <f>O107*$B$1/10</f>
+        <v>26.096699999999998</v>
+      </c>
+      <c r="Q107" s="18">
+        <f>(($J$47/COS(RADIANS(0))*$N$107)+(1/COS(RADIANS(180-165))*$P$107))</f>
+        <v>51.700128141963091</v>
+      </c>
+      <c r="R107" s="37"/>
+      <c r="S107" s="26">
+        <v>58.39</v>
+      </c>
+      <c r="T107" s="15">
+        <f>S107*$E$1/10</f>
+        <v>15.759460999999998</v>
+      </c>
+      <c r="U107" s="26">
+        <v>63.39</v>
+      </c>
+      <c r="V107" s="6">
+        <f>U107*$E$1/10</f>
+        <v>17.108961000000001</v>
+      </c>
+      <c r="W107" s="14">
+        <f>(($J$45/COS(RADIANS(0))*T107)+(1/COS(RADIANS(180-165))*V107))</f>
+        <v>31.333883779329351</v>
+      </c>
+      <c r="X107" s="38"/>
+    </row>
+    <row r="108" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B108" s="36"/>
+      <c r="C108" s="37"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="37"/>
+      <c r="K108" s="37"/>
+      <c r="L108" s="37"/>
+      <c r="M108" s="37"/>
+      <c r="N108" s="37"/>
+      <c r="O108" s="37"/>
+      <c r="P108" s="37"/>
+      <c r="Q108" s="37"/>
+      <c r="R108" s="37"/>
+      <c r="S108" s="37"/>
+      <c r="T108" s="37"/>
+      <c r="U108" s="37"/>
+      <c r="V108" s="37"/>
+      <c r="W108" s="37"/>
+      <c r="X108" s="38"/>
+    </row>
+    <row r="109" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="36"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="37"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="37"/>
+      <c r="K109" s="37"/>
+      <c r="L109" s="37"/>
+      <c r="M109" s="37"/>
+      <c r="N109" s="37"/>
+      <c r="O109" s="37"/>
+      <c r="P109" s="37"/>
+      <c r="Q109" s="37"/>
+      <c r="R109" s="37"/>
+      <c r="S109" s="37"/>
+      <c r="T109" s="37"/>
+      <c r="U109" s="37"/>
+      <c r="V109" s="37"/>
+      <c r="W109" s="37"/>
+      <c r="X109" s="38"/>
+    </row>
+    <row r="110" spans="2:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="36"/>
+      <c r="C110" s="37"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="37"/>
+      <c r="K110" s="37"/>
+      <c r="L110" s="37"/>
+      <c r="M110" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q110" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R110" s="37"/>
+      <c r="S110" s="7"/>
+      <c r="T110" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U110" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V110" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="W110" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="X110" s="38"/>
+    </row>
+    <row r="111" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="36"/>
+      <c r="C111" s="37"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="37"/>
+      <c r="K111" s="37"/>
+      <c r="L111" s="37"/>
+      <c r="M111" s="27"/>
+      <c r="N111" s="20">
+        <v>463.5</v>
+      </c>
+      <c r="O111" s="21">
+        <v>454.5</v>
+      </c>
+      <c r="P111" s="25">
+        <f>(N111-O111)*D102</f>
+        <v>88.211496483758523</v>
+      </c>
+      <c r="Q111" s="23">
+        <f>P111*10^3/$Q$88</f>
+        <v>1640.2685438403378</v>
+      </c>
+      <c r="R111" s="37"/>
+      <c r="S111" s="24"/>
+      <c r="T111" s="20">
+        <v>405</v>
+      </c>
+      <c r="U111" s="21">
+        <v>400</v>
+      </c>
+      <c r="V111" s="22">
+        <f>(T111-U111)*D102</f>
+        <v>49.006386935421403</v>
+      </c>
+      <c r="W111" s="23">
+        <f>V111*10^3/$W$88</f>
+        <v>1494.6842497603852</v>
+      </c>
+      <c r="X111" s="38"/>
+    </row>
+    <row r="112" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B112" s="36"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="37"/>
+      <c r="K112" s="37"/>
+      <c r="L112" s="37"/>
+      <c r="M112" s="37"/>
+      <c r="N112" s="37"/>
+      <c r="O112" s="37"/>
+      <c r="P112" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q112" s="37"/>
+      <c r="R112" s="37"/>
+      <c r="S112" s="37"/>
+      <c r="T112" s="37"/>
+      <c r="U112" s="37"/>
+      <c r="V112" s="37"/>
+      <c r="W112" s="37"/>
+      <c r="X112" s="38"/>
+    </row>
+    <row r="113" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B113" s="36"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="37"/>
+      <c r="K113" s="37"/>
+      <c r="L113" s="37"/>
+      <c r="M113" s="37"/>
+      <c r="N113" s="37"/>
+      <c r="O113" s="37"/>
+      <c r="P113" s="37"/>
+      <c r="Q113" s="37"/>
+      <c r="R113" s="37"/>
+      <c r="S113" s="37"/>
+      <c r="T113" s="37"/>
+      <c r="U113" s="37"/>
+      <c r="V113" s="37"/>
+      <c r="W113" s="37"/>
+      <c r="X113" s="38"/>
+    </row>
+    <row r="114" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B114" s="36"/>
+      <c r="C114" s="37"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="37"/>
+      <c r="K114" s="37"/>
+      <c r="L114" s="37"/>
+      <c r="M114" s="37"/>
+      <c r="N114" s="37"/>
+      <c r="O114" s="37"/>
+      <c r="P114" s="37"/>
+      <c r="Q114" s="37"/>
+      <c r="R114" s="37"/>
+      <c r="S114" s="37"/>
+      <c r="T114" s="37"/>
+      <c r="U114" s="37"/>
+      <c r="V114" s="37"/>
+      <c r="W114" s="37"/>
+      <c r="X114" s="38"/>
+    </row>
+    <row r="115" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="75"/>
+      <c r="C115" s="76"/>
+      <c r="D115" s="76"/>
+      <c r="E115" s="76"/>
+      <c r="F115" s="76"/>
+      <c r="G115" s="76"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
+      <c r="J115" s="76"/>
+      <c r="K115" s="76"/>
+      <c r="L115" s="76"/>
+      <c r="M115" s="76"/>
+      <c r="N115" s="76"/>
+      <c r="O115" s="76"/>
+      <c r="P115" s="76"/>
+      <c r="Q115" s="76"/>
+      <c r="R115" s="76"/>
+      <c r="S115" s="76"/>
+      <c r="T115" s="76"/>
+      <c r="U115" s="76"/>
+      <c r="V115" s="76"/>
+      <c r="W115" s="76"/>
+      <c r="X115" s="77"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Analysis update: new scripts     * CrossSection_RelMeth.py: for calculation using the relative method; using PlotData.py allows to choose between ploting only My cross-sections or plotting average of my cross-sections alognside other authors and Talys;     * MergeRBS.py: for merging RBS data files from different irradiations of the same beam energy;     * PlotTotalCurrent.py: now allows to plot the total beam current during each irradiation in the same canvas; auxiliar function defined in PlotData.py;     * RBS files for Ebeam=4.7MeV were corrected to be properly read;     * SimNRA simulations were performed to assess the targets thicknesses;
</commit_message>
<xml_diff>
--- a/CNA/RBS-TargetsAnalysis-CNA.xlsx
+++ b/CNA/RBS-TargetsAnalysis-CNA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="37">
   <si>
     <t>g/cm^3</t>
   </si>
@@ -1146,11 +1146,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1721889552"/>
-        <c:axId val="-1721890640"/>
+        <c:axId val="-81893088"/>
+        <c:axId val="-81887104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1721889552"/>
+        <c:axId val="-81893088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,12 +1263,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721890640"/>
+        <c:crossAx val="-81887104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1721890640"/>
+        <c:axId val="-81887104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1381,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721889552"/>
+        <c:crossAx val="-81893088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1598,11 +1598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1721894992"/>
-        <c:axId val="-1721888464"/>
+        <c:axId val="-81892544"/>
+        <c:axId val="-81897440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1721894992"/>
+        <c:axId val="-81892544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,12 +1715,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721888464"/>
+        <c:crossAx val="-81897440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1721888464"/>
+        <c:axId val="-81897440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,7 +1833,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721894992"/>
+        <c:crossAx val="-81892544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2050,11 +2050,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1721885200"/>
-        <c:axId val="-1721897168"/>
+        <c:axId val="-81888736"/>
+        <c:axId val="-81896352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1721885200"/>
+        <c:axId val="-81888736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,12 +2167,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721897168"/>
+        <c:crossAx val="-81896352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1721897168"/>
+        <c:axId val="-81896352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,7 +2285,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721885200"/>
+        <c:crossAx val="-81888736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2502,11 +2502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1721887920"/>
-        <c:axId val="-1721898800"/>
+        <c:axId val="-81884384"/>
+        <c:axId val="-81888192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1721887920"/>
+        <c:axId val="-81884384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2619,12 +2619,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721898800"/>
+        <c:crossAx val="-81888192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1721898800"/>
+        <c:axId val="-81888192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2737,7 +2737,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721887920"/>
+        <c:crossAx val="-81884384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2956,10 +2956,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sn+Al targets'!$L$81:$L$86</c:f>
+              <c:f>'Sn+Al targets'!$L$81:$L$85</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>317.5</c:v>
                 </c:pt>
@@ -2969,7 +2969,7 @@
                 <c:pt idx="2">
                   <c:v>378</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>434</c:v>
                 </c:pt>
               </c:numCache>
@@ -2977,10 +2977,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sn+Al targets'!$K$81:$K$86</c:f>
+              <c:f>'Sn+Al targets'!$K$81:$K$85</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3385.2787056917609</c:v>
                 </c:pt>
@@ -2991,12 +2991,9 @@
                   <c:v>4062.3537014991889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4085.8467891300279</c:v>
+                  <c:v>4543.3579823269692</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4543.3579823269692</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>4606.2280993468812</c:v>
                 </c:pt>
               </c:numCache>
@@ -3012,11 +3009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1721898256"/>
-        <c:axId val="-1721886832"/>
+        <c:axId val="-81895808"/>
+        <c:axId val="-81886560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1721898256"/>
+        <c:axId val="-81895808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,12 +3126,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721886832"/>
+        <c:crossAx val="-81886560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1721886832"/>
+        <c:axId val="-81886560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3247,7 +3244,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721898256"/>
+        <c:crossAx val="-81895808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3514,11 +3511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1602602544"/>
-        <c:axId val="-1602608528"/>
+        <c:axId val="-81886016"/>
+        <c:axId val="-166866624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1602602544"/>
+        <c:axId val="-81886016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,12 +3628,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1602608528"/>
+        <c:crossAx val="-166866624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1602608528"/>
+        <c:axId val="-166866624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3749,7 +3746,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1602602544"/>
+        <c:crossAx val="-81886016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7594,14 +7591,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M111" sqref="M111"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -10435,12 +10432,12 @@
     <row r="83" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B83" s="36"/>
       <c r="C83" s="37"/>
-      <c r="D83" s="37" t="e">
-        <f t="array" ref="D83:E86">LINEST(K81:K86,L81:L86,TRUE,TRUE)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E83" s="37" t="e">
-        <v>#VALUE!</v>
+      <c r="D83" s="37">
+        <f t="array" ref="D83:E86">LINEST(K81:K84,L81:L84,TRUE,TRUE)</f>
+        <v>10.028282738820089</v>
+      </c>
+      <c r="E83" s="37">
+        <v>215.99440361817187</v>
       </c>
       <c r="F83" s="37"/>
       <c r="G83" s="31" t="s">
@@ -10479,31 +10476,33 @@
     <row r="84" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B84" s="36"/>
       <c r="C84" s="37"/>
-      <c r="D84" s="37" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E84" s="37" t="e">
-        <v>#VALUE!</v>
+      <c r="D84" s="37">
+        <v>0.52999498018827829</v>
+      </c>
+      <c r="E84" s="37">
+        <v>196.90374545342524</v>
       </c>
       <c r="F84" s="37"/>
-      <c r="G84" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H84" s="40">
-        <v>14</v>
-      </c>
-      <c r="I84" s="40">
-        <v>28.09</v>
-      </c>
-      <c r="J84" s="49">
-        <f t="shared" si="8"/>
-        <v>0.86932910407021868</v>
-      </c>
-      <c r="K84" s="66">
-        <f t="shared" si="9"/>
-        <v>4085.8467891300279</v>
-      </c>
-      <c r="L84" s="41"/>
+      <c r="G84" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="42">
+        <v>50</v>
+      </c>
+      <c r="I84" s="42">
+        <v>116</v>
+      </c>
+      <c r="J84" s="43">
+        <f>((SQRT(1-(1/I84)^2*SIN(RADIANS(165))^2)+1/I84*COS(RADIANS(165)))/(1+1/I84))^2</f>
+        <v>0.96667191113339779</v>
+      </c>
+      <c r="K84" s="67">
+        <f>$D$80*1000*J84</f>
+        <v>4543.3579823269692</v>
+      </c>
+      <c r="L84" s="47">
+        <v>434</v>
+      </c>
       <c r="M84" s="37"/>
       <c r="N84" s="37"/>
       <c r="O84" s="37"/>
@@ -10517,36 +10516,34 @@
       <c r="W84" s="37"/>
       <c r="X84" s="38"/>
     </row>
-    <row r="85" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="36"/>
       <c r="C85" s="37"/>
-      <c r="D85" s="37" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E85" s="37" t="e">
-        <v>#VALUE!</v>
+      <c r="D85" s="37">
+        <v>0.99444478282660387</v>
+      </c>
+      <c r="E85" s="37">
+        <v>45.790155400265043</v>
       </c>
       <c r="F85" s="37"/>
-      <c r="G85" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="H85" s="42">
-        <v>50</v>
-      </c>
-      <c r="I85" s="42">
-        <v>116</v>
-      </c>
-      <c r="J85" s="43">
+      <c r="G85" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="H85" s="46">
+        <v>78</v>
+      </c>
+      <c r="I85" s="46">
+        <v>195.1</v>
+      </c>
+      <c r="J85" s="50">
         <f>((SQRT(1-(1/I85)^2*SIN(RADIANS(165))^2)+1/I85*COS(RADIANS(165)))/(1+1/I85))^2</f>
-        <v>0.96667191113339779</v>
-      </c>
-      <c r="K85" s="67">
-        <f t="shared" si="9"/>
-        <v>4543.3579823269692</v>
-      </c>
-      <c r="L85" s="47">
-        <v>434</v>
-      </c>
+        <v>0.9800485317759321</v>
+      </c>
+      <c r="K85" s="68">
+        <f>$D$80*1000*J85</f>
+        <v>4606.2280993468812</v>
+      </c>
+      <c r="L85" s="48"/>
       <c r="M85" s="37"/>
       <c r="N85" s="37"/>
       <c r="O85" s="37"/>
@@ -10563,31 +10560,13 @@
     <row r="86" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="36"/>
       <c r="C86" s="37"/>
-      <c r="D86" s="37" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E86" s="37" t="e">
-        <v>#VALUE!</v>
+      <c r="D86" s="37">
+        <v>358.02192849956941</v>
+      </c>
+      <c r="E86" s="37">
+        <v>2</v>
       </c>
       <c r="F86" s="37"/>
-      <c r="G86" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="H86" s="46">
-        <v>78</v>
-      </c>
-      <c r="I86" s="46">
-        <v>195.1</v>
-      </c>
-      <c r="J86" s="50">
-        <f>((SQRT(1-(1/I86)^2*SIN(RADIANS(165))^2)+1/I86*COS(RADIANS(165)))/(1+1/I86))^2</f>
-        <v>0.9800485317759321</v>
-      </c>
-      <c r="K86" s="68">
-        <f t="shared" si="9"/>
-        <v>4606.2280993468812</v>
-      </c>
-      <c r="L86" s="48"/>
       <c r="M86" s="37"/>
       <c r="N86" s="37"/>
       <c r="O86" s="37"/>

</xml_diff>

<commit_message>
Analysis update (accumulation):     * Fits.py: added function NpeakNoLin and FitNpeakNoLin to perform acumulation fit without linear trend consideration (bad results);         - FitNpeakHalfLifeSDD: included L-lines fit;     * Accumulation_Fit_HalfLife_SDD.py: included linear trend consideration (better results for N0 and half-life);     * RBS-TargetsAnalysis-CNA.xlsx: minor corrections slighly changed calculated thickness of target used at Ebeam=5.0 MeV;
</commit_message>
<xml_diff>
--- a/CNA/RBS-TargetsAnalysis-CNA.xlsx
+++ b/CNA/RBS-TargetsAnalysis-CNA.xlsx
@@ -1146,11 +1146,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81893088"/>
-        <c:axId val="-81887104"/>
+        <c:axId val="1319614192"/>
+        <c:axId val="1319609840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81893088"/>
+        <c:axId val="1319614192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,12 +1263,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81887104"/>
+        <c:crossAx val="1319609840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81887104"/>
+        <c:axId val="1319609840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1381,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81893088"/>
+        <c:crossAx val="1319614192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1598,11 +1598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81892544"/>
-        <c:axId val="-81897440"/>
+        <c:axId val="1319616368"/>
+        <c:axId val="1319611472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81892544"/>
+        <c:axId val="1319616368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,12 +1715,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81897440"/>
+        <c:crossAx val="1319611472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81897440"/>
+        <c:axId val="1319611472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,7 +1833,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81892544"/>
+        <c:crossAx val="1319616368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2050,11 +2050,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81888736"/>
-        <c:axId val="-81896352"/>
+        <c:axId val="1319612016"/>
+        <c:axId val="1319614736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81888736"/>
+        <c:axId val="1319612016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,12 +2167,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81896352"/>
+        <c:crossAx val="1319614736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81896352"/>
+        <c:axId val="1319614736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,7 +2285,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81888736"/>
+        <c:crossAx val="1319612016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2502,11 +2502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81884384"/>
-        <c:axId val="-81888192"/>
+        <c:axId val="1319615280"/>
+        <c:axId val="1319615824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81884384"/>
+        <c:axId val="1319615280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2619,12 +2619,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81888192"/>
+        <c:crossAx val="1319615824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81888192"/>
+        <c:axId val="1319615824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2737,7 +2737,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81884384"/>
+        <c:crossAx val="1319615280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3009,11 +3009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81895808"/>
-        <c:axId val="-81886560"/>
+        <c:axId val="1319616912"/>
+        <c:axId val="1319618000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81895808"/>
+        <c:axId val="1319616912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,12 +3126,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81886560"/>
+        <c:crossAx val="1319618000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81886560"/>
+        <c:axId val="1319618000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3244,7 +3244,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81895808"/>
+        <c:crossAx val="1319616912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3511,11 +3511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81886016"/>
-        <c:axId val="-166866624"/>
+        <c:axId val="1319618544"/>
+        <c:axId val="1096201808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81886016"/>
+        <c:axId val="1319618544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3628,12 +3628,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166866624"/>
+        <c:crossAx val="1096201808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-166866624"/>
+        <c:axId val="1096201808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3746,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81886016"/>
+        <c:crossAx val="1319618544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7591,8 +7591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T112" sqref="T112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7978,7 +7978,7 @@
       <c r="W10" s="37"/>
       <c r="X10" s="38"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="36"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -10406,11 +10406,11 @@
         <v>15.999000000000001</v>
       </c>
       <c r="J82" s="55">
-        <f t="shared" ref="J82:J84" si="8">((SQRT(1-(1/I82)^2*SIN(RADIANS(165))^2)+1/I82*COS(RADIANS(165)))/(1+1/I82))^2</f>
+        <f t="shared" ref="J82:J83" si="8">((SQRT(1-(1/I82)^2*SIN(RADIANS(165))^2)+1/I82*COS(RADIANS(165)))/(1+1/I82))^2</f>
         <v>0.78185798881983415</v>
       </c>
       <c r="K82" s="64">
-        <f t="shared" ref="K82:K86" si="9">$D$80*1000*J82</f>
+        <f t="shared" ref="K82:K83" si="9">$D$80*1000*J82</f>
         <v>3674.7325474532204</v>
       </c>
       <c r="L82" s="56">
@@ -10789,12 +10789,12 @@
         <v>425.5</v>
       </c>
       <c r="P92" s="25">
-        <f>(N92-O92)*10.028</f>
-        <v>85.238</v>
+        <f>(N92-O92)*D83</f>
+        <v>85.240403279970749</v>
       </c>
       <c r="Q92" s="23">
         <f>P92*10^3/$Q$88</f>
-        <v>1584.9771935974929</v>
+        <v>1585.021881928325</v>
       </c>
       <c r="R92" s="37"/>
       <c r="S92" s="24"/>
@@ -10805,12 +10805,12 @@
         <v>373.5</v>
       </c>
       <c r="V92" s="22">
-        <f>(T92-U92)*10.028</f>
-        <v>45.126000000000005</v>
+        <f>(T92-U92)*D83</f>
+        <v>45.127272324690395</v>
       </c>
       <c r="W92" s="23">
         <f>V92*10^3/$W$88</f>
-        <v>1376.3332837323596</v>
+        <v>1376.3720893614668</v>
       </c>
       <c r="X92" s="38"/>
     </row>
@@ -11327,7 +11327,7 @@
         <v>17.108961000000001</v>
       </c>
       <c r="W107" s="14">
-        <f>(($J$45/COS(RADIANS(0))*T107)+(1/COS(RADIANS(180-165))*V107))</f>
+        <f>(($J$102/COS(RADIANS(0))*T107)+(1/COS(RADIANS(180-165))*V107))</f>
         <v>31.333883779329351</v>
       </c>
       <c r="X107" s="38"/>
@@ -11449,24 +11449,24 @@
         <v>88.211496483758523</v>
       </c>
       <c r="Q111" s="23">
-        <f>P111*10^3/$Q$88</f>
-        <v>1640.2685438403378</v>
+        <f>P111*10^3/$Q$107</f>
+        <v>1706.2142716849573</v>
       </c>
       <c r="R111" s="37"/>
       <c r="S111" s="24"/>
       <c r="T111" s="20">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="U111" s="21">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="V111" s="22">
         <f>(T111-U111)*D102</f>
-        <v>49.006386935421403</v>
+        <v>29.40383216125284</v>
       </c>
       <c r="W111" s="23">
-        <f>V111*10^3/$W$88</f>
-        <v>1494.6842497603852</v>
+        <f>V111*10^3/$W$107</f>
+        <v>938.40369002230921</v>
       </c>
       <c r="X111" s="38"/>
     </row>

</xml_diff>